<commit_message>
Adding functionality to incorporate transmission pair data
</commit_message>
<xml_diff>
--- a/tabular/iyer/hiv_pairs_dr_patient.xlsx
+++ b/tabular/iyer/hiv_pairs_dr_patient.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9620" yWindow="8100" windowWidth="13640" windowHeight="10800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="26">
   <si>
     <t>Sex</t>
   </si>
@@ -88,6 +89,15 @@
   </si>
   <si>
     <t>South Africa</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>sex</t>
   </si>
 </sst>
 </file>
@@ -156,8 +166,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -192,7 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -207,6 +229,12 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -221,6 +249,12 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="A2:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -746,4 +780,201 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="A1:C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>